<commit_message>
update 0518 avg en
</commit_message>
<xml_diff>
--- a/3000-40960-tfEN-1.8160/平均时频熵.xlsx
+++ b/3000-40960-tfEN-1.8160/平均时频熵.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\58497_000\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\学习\2219铝合金焊接\代码-电信号计算\2219-welding-signal\3000-40960-tfEN-1.8160\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="984" yWindow="0" windowWidth="22056" windowHeight="9948"/>
+    <workbookView xWindow="1968" yWindow="0" windowWidth="22056" windowHeight="9948"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -317,11 +313,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="623603744"/>
-        <c:axId val="864485680"/>
+        <c:axId val="-2079858224"/>
+        <c:axId val="-2079849520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="623603744"/>
+        <c:axId val="-2079858224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -364,7 +360,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="864485680"/>
+        <c:crossAx val="-2079849520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -372,7 +368,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="864485680"/>
+        <c:axId val="-2079849520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -423,7 +419,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="623603744"/>
+        <c:crossAx val="-2079858224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1065,15 +1061,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
+      <xdr:colOff>601980</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>41910</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
+      <xdr:colOff>297180</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>41910</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1361,7 +1357,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="A2" sqref="A2:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>

</xml_diff>